<commit_message>
Modified course and requisite importation, data
- Renamed and aggregated course and requisite importation, moved them into a single file
- Modified course information
</commit_message>
<xml_diff>
--- a/app/data/chemistry.xlsx
+++ b/app/data/chemistry.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lambe\OneDrive\Documents\Courses\2023-2024\Semester 2\COMP3901\FST-Degree-Planner\project\app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lambe\OneDrive\Documents\Courses\2023-2024\Semester 2\COMP3901\FST-Degree-Planner\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3BBF69-A4A3-4B82-9EF7-F0B25890C2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6C877C-A730-44AA-99C9-6D1E4AD0CF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
     <sheet name="Majors" sheetId="4" r:id="rId2"/>
-    <sheet name="Minors" sheetId="5" r:id="rId3"/>
+    <sheet name="Programmes" sheetId="6" r:id="rId3"/>
+    <sheet name="Minors" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="322">
   <si>
     <t>LEVEL</t>
   </si>
@@ -64,9 +65,6 @@
   </si>
   <si>
     <t>RECOMMENDED_COURSES</t>
-  </si>
-  <si>
-    <t>Microbiology</t>
   </si>
   <si>
     <t>NOTES</t>
@@ -3024,12 +3022,307 @@
   <si>
     <t>ANTI-REQUISITE</t>
   </si>
+  <si>
+    <t>Applied Chemistry</t>
+  </si>
+  <si>
+    <t>Environmental Chemistry</t>
+  </si>
+  <si>
+    <t>Food Chemistry</t>
+  </si>
+  <si>
+    <t>General Chemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Environmental Chemistry</t>
+  </si>
+  <si>
+    <t>Food Processing</t>
+  </si>
+  <si>
+    <t>Industrial Chemistry</t>
+  </si>
+  <si>
+    <t>LEVEL1_CREDITS_REQUIRED</t>
+  </si>
+  <si>
+    <t>ADVANCED_CREDITS</t>
+  </si>
+  <si>
+    <t>MINOR</t>
+  </si>
+  <si>
+    <t>Major requires thirty-five (35) credits of specialized Food Chemistry courses 
+supported by 10 prerequisite credits of General Chemistry (CHEM2010, 
+CHEM2011, CHEM2210, and CHEM2211). These prerequisite courses can 
+contribute towards a minor in General Chemistry.</t>
+  </si>
+  <si>
+    <t>Minor consists of 16 compulsory advanced credits. CHEM3402 examines the 
+operations of selected chemical industries and includes an internship within an 
+approved chemical industry. CHEM3401 deals with project management while 
+CHEM3403 covers the unit operations of chemical industries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEM1810,CHEM1820,CHEM1910 ,CHEM1920, CHEM1811,CHEM1911(or CHEM1901 + CHEM1902)
+CHEM3401,CHEM3402,CHEM3403 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CHEM1810,CHEM1820,CHEM1910,
+CHEM1920,CHEM1811,CHEM1911(or CHEM1901 + CHEM1902),CHEM2420,CHEM2421,CHEM3610 
+CHEM3611,CHEM3612 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">None
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CHEM1810,CHEM1820,CHEM1910,
+CHEM1920,CHEM1811,CHEM1911
+(or CHEM1901 + CHEM1902),
+MATH - 6 credits from any Level I Mathematics courses,
+CHEM2010,CHEM2011,CHEM2210,
+CHEM2211,CHEM2510
+CHEM2511,CHEM2512,CHEM2420,
+CHEM2421,CHEM3010,CHEM3011 
+CHEM340,CHEM3510CHEM3511
+CHEM3512,CHEM3513 and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                 The major requires 25 credits of specified Environmental courses along with 6 
+credits from Level 2 or 3 approved environment-related electives; an additional 
+4 credits from Level 2 laboratory electives are also required. There are 14 credits 
+of defined prerequisite courses (CHEM2010, CHEM2011, CHEM2110, 
+CHEM2210, and CHEM2310)       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CHEM1810,CHEM1820,CHEM1910, 
+CHEM1920, CHEM1811,CHEM1911,
+(or CHEM1901 + CHEM1902),
+MATH - 6 credits from any Level 1 Mathematics courses , CHEM2010, CHEM2011, CHEM2110, CHEM2210, CHEM2310 CHEM2420, 
+CHEM2421, four credits from:(CHEM2111 CHEM2211,CHEM2311),CHEM3010,
+CHEM3011, CHEM3402,CHEM3610
+CHEM3611, CHEM3612 and any six additional credits from:(CHEM3621,CHEM3711,
+BIOL2402,BIOL2403,
+BIOL3405,BIOL3406,
+BIOL3407,BIOL3408,
+BIOL3409,BIOL3410,
+BOTN3403,BOTN3404,
+BOTN3405,BIOL2402,
+BIOL2403,GEOG2131,
+GEOG2232,GEOG3132,
+GGEO2233,GGEO3232,
+GGEO3233,PHYS2701,
+PHYS3701, PHYS3661,
+PHYS3671,PHYS3681)</t>
+  </si>
+  <si>
+    <t>Major requires 20 Level 2 credits consisting of core courses in Analytical, Inorganic, 
+Organic and Physical Chemistry (A, I, O and P) and include 8 credits in laboratory 
+courses which span the four sub-disciplines. At Level 3, students take 10 credits of core 
+chemistry, inclusive of 4 credits in laboratory courses. An additional 9 credits in chemistry 
+electives are required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CHEM1810,CHEM1820,CHEM1910,
+CHEM1920, CHEM1811, 
+(or CHEM1901 + CHEM1902)
+and 
+MATH - 6 credits from any Level 1 Mathematics courses 
+(taken in Semester 1 and/or Semester 2)
+CHEM2010,CHEM2011,CHEM2110,
+CHEM2111,CHEM2211,CHEM2310,
+CHEM2311,at least six credits from:(CHEM3010, CHEM3110, CHEM3210,CHEM3310), at least four credits from:( CHEM3011,
+CHEM3111,CHEM3211 CHEM3311) and least three credits from:(CHEM3112,CHEM3212 CHEM3213, CHEM3312,CHEM3313) and six additional credits from:(CHEM2420 ,CHEM2421,CHEM2510,CHEM2511,CHEM2512,CHEM2513,CHEM3112,CHEM3113,CHEM3402,CHEM3510,CHEM3512,CHEM3610,CHEM3612,CHEM3111,CHEM3211,CHEM3311,CHEM3511,CHEM3611,CHEM3621)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEM1810 ,CHEM1820 ,CHEM1910
+CHEM1920,CHEM1811,CHEM1911(or CHEM1901 + CHEM1902), CHEM3510,CHEM3511,
+CHEM3512 and at least seven credits from:(CHEM2010,CHEM2011,CHEM2210,CHEM2211,CHEM2310, CHEM2311,CHEM2420 
+CHEM2421,CHEM3010,CHEM3011,
+CHEM3210,CHEM3513 )
+</t>
+  </si>
+  <si>
+    <t>Minor consists of 16 credits of Advanced courses. The required Level 3 courses 
+explore the chemistry of food components while the additional 7 credits may be 
+selected from Level 2 or Level 3 courses that cover central areas of organic and 
+physical chemistry, chemical analysis, water treatment, instrumental methods or 
+food safety.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+CHEM1810,CHEM1820,CHEM1910,
+CHEM1920,CHEM1811,CHEM1911
+(or CHEM1901 + CHEM1902)
+CHEM2510,CHEM2511,CHEM2512 and at least seven credits from:(CHEM2010,CHEM2011,CHEM2210,
+CHEM2211,CHEM2310,CHEM2311,
+CHEM2420,CHEM2421,CHEM3010,
+CHEM3011,CHEM3210,CHEM3513 )</t>
+  </si>
+  <si>
+    <t>Minor consists of 16 Advanced (Level 2 and Level 3) credits. The compulsory 
+Level 2 courses (9 credits) explore the theory of various food processing 
+technologies, laboratory analyses of raw and processed foods as well as pilot scale 
+processing of local foods. The additional 7 credits may be selected from Level 2 
+or Level 3 courses that cover central areas of physical chemistry, water treatment, 
+industrial chemistry, unit operations, food safety and the integration of business and 
+management in the food industry.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CHEM1810,CHEM1820 CHEM1910,
+CHEM1920,CHEM1811,CHEM1911 
+(or CHEM1901 + CHEM1902),CHEM2010 
+CHEM2011,CHEM2110,CHEM2210,CHEM2310 and at leasr two credits from:(CHEM2111,CHEM2211,CHEM2311 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The General Chemistry minor gives students a foundation in analytical chemistry 
+and the other traditional chemistry sub-disciplines (inorganic, organic and physical 
+chemistry). The minor comprises 12 credits of theory and 4 credits of laboratory 
+from Level 2 core courses </t>
+  </si>
+  <si>
+    <t>COURSE_OPTIONS</t>
+  </si>
+  <si>
+    <t>NUMBER_REQUIRED</t>
+  </si>
+  <si>
+    <t>COURSE_ALTERNATIVES</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>Chemistry and Management (B.Sc.)</t>
+  </si>
+  <si>
+    <t>ADVANCED_CREDITS_REQUIRED</t>
+  </si>
+  <si>
+    <t>COURSE_CODE</t>
+  </si>
+  <si>
+    <t>ALTERNATIVES</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>CREDITS_REQUIRED</t>
+  </si>
+  <si>
+    <t>CHEM1911</t>
+  </si>
+  <si>
+    <t>CHEM1901 + CHEM1902</t>
+  </si>
+  <si>
+    <t>CHEM1810, CHEM1820, CHEM1910, CHEM1920, CHEM1811, CHEM1911, STAT1001, ACCT1003, ACCT1005, ECON1000, ECON1012, PSYC1002, SOCI1002</t>
+  </si>
+  <si>
+    <t>MANDATORY_LEVEL1_COURSES</t>
+  </si>
+  <si>
+    <t>MANDATORY_ADVANCED_COURSES</t>
+  </si>
+  <si>
+    <t>PROGRAMME_COURSE_ALTERNATIVES</t>
+  </si>
+  <si>
+    <t>PROGRAMME_DEPARTMENTAL_REQUIREMENTS</t>
+  </si>
+  <si>
+    <t>PROGRAMME_COURSE_OPTIONS</t>
+  </si>
+  <si>
+    <t>COURSES_LIST</t>
+  </si>
+  <si>
+    <t>CHEM3010, CHEM3110, CHEM3210, CHEM3310</t>
+  </si>
+  <si>
+    <t>CHEM2010, CHEM2011, CHEM2110, CHEM2111, CHEM2210, CHEM2211, CHEM2310, CHEM2311, MKTG2001, MGMT2004, MGMT2008, MGMT2012, MGMT2021, MGMT2023, MGMT2026, MGMT3031, MGMT3058</t>
+  </si>
+  <si>
+    <t>Management Studies</t>
+  </si>
+  <si>
+    <t>2 or 3</t>
+  </si>
+  <si>
+    <t>CHEM2420, CHEM2421, CHEM2510, CHEM2511, CHEM2512, CHEM3111, CHEM3112, CHEM3211, CHEM3212, CHEM3213, CHEM3311, CHEM3312, CHEM3313, CHEM3402, CHEM3510, CHEM3511, CHEM3512, CHEM3513, CHEM3610, CHEM3611, CHEM3612, CHEM3621, CHEM3711</t>
+  </si>
+  <si>
+    <t>Electives
+Students must ensure that they satisfy the prerequisite courses required for entry to the electives of interest. In most instances, 12 Level 1 credits in the subject of interest are required. One or more advanced courses may also be needed.</t>
+  </si>
+  <si>
+    <t>OCCUPATIONAL AND ENVIRONMENTAL SAFETY AND HEALTH (B.Sc.)</t>
+  </si>
+  <si>
+    <t>BIOL1017, BIOL1262, BIOL1263, CHEM1810, CHEM1820, CHEM1910, CHEM1920, CHEM1811, CHEM1911, GEOG1231, GEOG1232, OESH1000, PSYC1002</t>
+  </si>
+  <si>
+    <t>MANDATORY_SUMMER_COURSES</t>
+  </si>
+  <si>
+    <t>OESH2000</t>
+  </si>
+  <si>
+    <t>CHEM2420 + CHEM2421 + CHEM3610</t>
+  </si>
+  <si>
+    <t>BIOL2403, BIOL2406, CHEM2010, CHEM2011, CHEM3010, CHEM3011, LANG3101, OESH3200, OESH3220, PHAL3306, OESH2000, OESH3010, OESH3020, OESH3030, OESH3040, OESH3100, OESH3210, MGMT3063</t>
+  </si>
+  <si>
+    <t>MDSC3200, OESH3430</t>
+  </si>
+  <si>
+    <t>SPECIAL CHEMISTRY (B.Sc.)</t>
+  </si>
+  <si>
+    <t>CHEMISTRY AND MANAGEMENT (B.Sc.)</t>
+  </si>
+  <si>
+    <t>CHEM1810, CHEM1820, CHEM1910, CHEM1920, CHEM1811, CHEM1911</t>
+  </si>
+  <si>
+    <t>1 or 2</t>
+  </si>
+  <si>
+    <t>CAPE Physics or equivalent is required</t>
+  </si>
+  <si>
+    <t>CHEM2010, CHEM2011, CHEM2110, CHEM2111, CHEM2210, CHEM2211, CHEM2310, CHEM2311, CHEM3010, CHEM3011, CHEM3110, CHEM3210, CHEM3310, CHEM3711</t>
+  </si>
+  <si>
+    <t>CHEM3111, CHEM3211, CHEM3311</t>
+  </si>
+  <si>
+    <t>CHEM2420, CHEM2421, CHEM2510, CHEM2511, CHEM2512, CHEM3111, CHEM3112, CHEM3211, CHEM3212, CHEM3213, CHEM3311, CHEM3312, CHEM3313, CHEM3402, CHEM3510, CHEM3511, CHEM3512, CHEM3610, CHEM3611, CHEM3612, CHEM3621</t>
+  </si>
+  <si>
+    <t>NUMBER_OF_COURSES_REQUIRED</t>
+  </si>
+  <si>
+    <t>!Chemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3058,7 +3351,7 @@
     <font>
       <sz val="8"/>
       <name val="Times New Roman"/>
-      <charset val="204"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3076,6 +3369,11 @@
       <sz val="10"/>
       <name val="Tw Cen MT"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3124,7 +3422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3178,6 +3476,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3485,24 +3789,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="39.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="60.44140625" style="1" customWidth="1"/>
     <col min="8" max="9" width="20.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.44140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="19.44140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="19.77734375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3513,25 +3818,25 @@
         <v>10</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>19</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>6</v>
@@ -3543,15 +3848,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D2" s="8">
         <v>0</v>
@@ -3563,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>3</v>
@@ -3575,21 +3880,21 @@
         <v>8</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>24</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -3601,7 +3906,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>3</v>
@@ -3613,21 +3918,21 @@
         <v>8</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>27</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -3639,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>3</v>
@@ -3651,7 +3956,7 @@
         <v>8</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>5</v>
@@ -3659,13 +3964,13 @@
     </row>
     <row r="5" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -3677,10 +3982,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>3</v>
@@ -3689,7 +3994,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>5</v>
@@ -3697,13 +4002,13 @@
     </row>
     <row r="6" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="C6" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -3715,7 +4020,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>3</v>
@@ -3727,7 +4032,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>5</v>
@@ -3735,13 +4040,13 @@
     </row>
     <row r="7" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="C7" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -3753,7 +4058,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>3</v>
@@ -3765,7 +4070,7 @@
         <v>8</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>5</v>
@@ -3773,13 +4078,13 @@
     </row>
     <row r="8" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="C8" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -3791,10 +4096,10 @@
         <v>2</v>
       </c>
       <c r="G8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>3</v>
@@ -3803,7 +4108,7 @@
         <v>8</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>5</v>
@@ -3811,13 +4116,13 @@
     </row>
     <row r="9" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="C9" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -3829,7 +4134,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>3</v>
@@ -3841,7 +4146,7 @@
         <v>8</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>5</v>
@@ -3849,13 +4154,13 @@
     </row>
     <row r="10" spans="1:12" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>45</v>
-      </c>
       <c r="C10" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D10" s="4">
         <v>2</v>
@@ -3867,7 +4172,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>3</v>
@@ -3879,7 +4184,7 @@
         <v>8</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>5</v>
@@ -3887,13 +4192,13 @@
     </row>
     <row r="11" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="C11" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D11" s="4">
         <v>2</v>
@@ -3905,10 +4210,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>3</v>
@@ -3917,7 +4222,7 @@
         <v>8</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>5</v>
@@ -3925,13 +4230,13 @@
     </row>
     <row r="12" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="C12" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D12" s="4">
         <v>2</v>
@@ -3943,7 +4248,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>3</v>
@@ -3955,7 +4260,7 @@
         <v>8</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>5</v>
@@ -3963,13 +4268,13 @@
     </row>
     <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="C13" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D13" s="4">
         <v>2</v>
@@ -3981,10 +4286,10 @@
         <v>2</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>3</v>
@@ -3993,7 +4298,7 @@
         <v>8</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>5</v>
@@ -4001,13 +4306,13 @@
     </row>
     <row r="14" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>53</v>
-      </c>
       <c r="C14" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D14" s="4">
         <v>2</v>
@@ -4019,7 +4324,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>3</v>
@@ -4031,7 +4336,7 @@
         <v>8</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>5</v>
@@ -4039,13 +4344,13 @@
     </row>
     <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="C15" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D15" s="4">
         <v>2</v>
@@ -4057,10 +4362,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>3</v>
@@ -4069,7 +4374,7 @@
         <v>8</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>5</v>
@@ -4077,13 +4382,13 @@
     </row>
     <row r="16" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="C16" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D16" s="4">
         <v>2</v>
@@ -4095,7 +4400,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>3</v>
@@ -4107,7 +4412,7 @@
         <v>8</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>5</v>
@@ -4115,13 +4420,13 @@
     </row>
     <row r="17" spans="1:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>70</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D17" s="4">
         <v>2</v>
@@ -4133,10 +4438,10 @@
         <v>2</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>3</v>
@@ -4145,7 +4450,7 @@
         <v>7</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>5</v>
@@ -4153,13 +4458,13 @@
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="C18" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D18" s="4">
         <v>2</v>
@@ -4171,7 +4476,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>3</v>
@@ -4183,7 +4488,7 @@
         <v>8</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>5</v>
@@ -4191,13 +4496,13 @@
     </row>
     <row r="19" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="C19" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D19" s="4">
         <v>2</v>
@@ -4209,10 +4514,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>3</v>
@@ -4221,7 +4526,7 @@
         <v>8</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>5</v>
@@ -4229,13 +4534,13 @@
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>76</v>
-      </c>
       <c r="C20" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D20" s="4">
         <v>2</v>
@@ -4247,10 +4552,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>3</v>
@@ -4259,21 +4564,21 @@
         <v>8</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>78</v>
-      </c>
       <c r="C21" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D21" s="4">
         <v>2</v>
@@ -4285,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>3</v>
@@ -4297,7 +4602,7 @@
         <v>8</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>5</v>
@@ -4305,13 +4610,13 @@
     </row>
     <row r="22" spans="1:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>80</v>
-      </c>
       <c r="C22" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D22" s="4">
         <v>2</v>
@@ -4323,10 +4628,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>3</v>
@@ -4335,7 +4640,7 @@
         <v>8</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>5</v>
@@ -4343,13 +4648,13 @@
     </row>
     <row r="23" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>88</v>
-      </c>
       <c r="C23" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D23" s="4">
         <v>2</v>
@@ -4361,7 +4666,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>3</v>
@@ -4373,7 +4678,7 @@
         <v>8</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>5</v>
@@ -4381,13 +4686,13 @@
     </row>
     <row r="24" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>90</v>
-      </c>
       <c r="C24" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D24" s="4">
         <v>3</v>
@@ -4399,7 +4704,7 @@
         <v>2</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>3</v>
@@ -4411,7 +4716,7 @@
         <v>8</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>5</v>
@@ -4419,13 +4724,13 @@
     </row>
     <row r="25" spans="1:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>92</v>
-      </c>
       <c r="C25" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D25" s="4">
         <v>3</v>
@@ -4437,10 +4742,10 @@
         <v>2</v>
       </c>
       <c r="G25" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>3</v>
@@ -4449,7 +4754,7 @@
         <v>8</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>5</v>
@@ -4457,13 +4762,13 @@
     </row>
     <row r="26" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>94</v>
-      </c>
       <c r="C26" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D26" s="4">
         <v>3</v>
@@ -4475,7 +4780,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>3</v>
@@ -4487,7 +4792,7 @@
         <v>8</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>5</v>
@@ -4495,13 +4800,13 @@
     </row>
     <row r="27" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>96</v>
-      </c>
       <c r="C27" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D27" s="4">
         <v>3</v>
@@ -4513,10 +4818,10 @@
         <v>2</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>3</v>
@@ -4525,7 +4830,7 @@
         <v>8</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>5</v>
@@ -4533,13 +4838,13 @@
     </row>
     <row r="28" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>98</v>
-      </c>
       <c r="C28" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D28" s="4">
         <v>3</v>
@@ -4551,7 +4856,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>3</v>
@@ -4563,7 +4868,7 @@
         <v>8</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>5</v>
@@ -4571,13 +4876,13 @@
     </row>
     <row r="29" spans="1:12" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>100</v>
-      </c>
       <c r="C29" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D29" s="4">
         <v>3</v>
@@ -4589,7 +4894,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>3</v>
@@ -4601,21 +4906,21 @@
         <v>8</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>102</v>
-      </c>
       <c r="C30" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D30" s="4">
         <v>3</v>
@@ -4627,10 +4932,10 @@
         <v>2</v>
       </c>
       <c r="G30" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>3</v>
@@ -4639,7 +4944,7 @@
         <v>8</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L30" s="4" t="s">
         <v>5</v>
@@ -4647,13 +4952,13 @@
     </row>
     <row r="31" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>104</v>
-      </c>
       <c r="C31" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D31" s="4">
         <v>3</v>
@@ -4665,7 +4970,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>3</v>
@@ -4677,21 +4982,21 @@
         <v>8</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>106</v>
-      </c>
       <c r="C32" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D32" s="4">
         <v>3</v>
@@ -4703,7 +5008,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>3</v>
@@ -4715,7 +5020,7 @@
         <v>8</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>5</v>
@@ -4723,13 +5028,13 @@
     </row>
     <row r="33" spans="1:12" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="C33" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D33" s="4">
         <v>3</v>
@@ -4741,7 +5046,7 @@
         <v>2</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>3</v>
@@ -4753,7 +5058,7 @@
         <v>8</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>5</v>
@@ -4761,13 +5066,13 @@
     </row>
     <row r="34" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="C34" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D34" s="4">
         <v>3</v>
@@ -4779,10 +5084,10 @@
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>3</v>
@@ -4791,7 +5096,7 @@
         <v>8</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>5</v>
@@ -4799,13 +5104,13 @@
     </row>
     <row r="35" spans="1:12" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="C35" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D35" s="4">
         <v>3</v>
@@ -4817,7 +5122,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>3</v>
@@ -4829,21 +5134,21 @@
         <v>8</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="C36" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D36" s="4">
         <v>3</v>
@@ -4855,7 +5160,7 @@
         <v>2</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>3</v>
@@ -4867,7 +5172,7 @@
         <v>8</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>5</v>
@@ -4875,13 +5180,13 @@
     </row>
     <row r="37" spans="1:12" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="C37" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D37" s="4">
         <v>3</v>
@@ -4893,7 +5198,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>3</v>
@@ -4905,7 +5210,7 @@
         <v>8</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>5</v>
@@ -4913,13 +5218,13 @@
     </row>
     <row r="38" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="C38" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D38" s="4">
         <v>3</v>
@@ -4931,7 +5236,7 @@
         <v>2</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>3</v>
@@ -4943,7 +5248,7 @@
         <v>8</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L38" s="4" t="s">
         <v>5</v>
@@ -4951,13 +5256,13 @@
     </row>
     <row r="39" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="C39" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D39" s="4">
         <v>3</v>
@@ -4969,7 +5274,7 @@
         <v>2</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>3</v>
@@ -4981,7 +5286,7 @@
         <v>8</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L39" s="4" t="s">
         <v>5</v>
@@ -4989,13 +5294,13 @@
     </row>
     <row r="40" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="C40" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D40" s="4">
         <v>3</v>
@@ -5007,7 +5312,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>3</v>
@@ -5019,21 +5324,21 @@
         <v>8</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L40" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="C41" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D41" s="4">
         <v>3</v>
@@ -5045,10 +5350,10 @@
         <v>2</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>3</v>
@@ -5057,7 +5362,7 @@
         <v>8</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>5</v>
@@ -5065,13 +5370,13 @@
     </row>
     <row r="42" spans="1:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="C42" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D42" s="4">
         <v>3</v>
@@ -5083,7 +5388,7 @@
         <v>2</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>3</v>
@@ -5095,7 +5400,7 @@
         <v>8</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>5</v>
@@ -5103,13 +5408,13 @@
     </row>
     <row r="43" spans="1:12" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="C43" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D43" s="4">
         <v>3</v>
@@ -5121,7 +5426,7 @@
         <v>2</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>3</v>
@@ -5133,21 +5438,21 @@
         <v>8</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L43" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="C44" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D44" s="4">
         <v>3</v>
@@ -5159,7 +5464,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>3</v>
@@ -5171,7 +5476,7 @@
         <v>8</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>5</v>
@@ -5179,13 +5484,13 @@
     </row>
     <row r="45" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="C45" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D45" s="4">
         <v>3</v>
@@ -5197,10 +5502,10 @@
         <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>3</v>
@@ -5209,7 +5514,7 @@
         <v>8</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>5</v>
@@ -5217,13 +5522,13 @@
     </row>
     <row r="46" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="C46" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D46" s="4">
         <v>3</v>
@@ -5235,7 +5540,7 @@
         <v>2</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>3</v>
@@ -5247,21 +5552,21 @@
         <v>8</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L46" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="C47" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D47" s="4">
         <v>3</v>
@@ -5273,7 +5578,7 @@
         <v>3</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>3</v>
@@ -5285,7 +5590,7 @@
         <v>8</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L47" s="4" t="s">
         <v>5</v>
@@ -5293,13 +5598,13 @@
     </row>
     <row r="48" spans="1:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="C48" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D48" s="4">
         <v>3</v>
@@ -5308,10 +5613,10 @@
         <v>6</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>3</v>
@@ -5323,7 +5628,7 @@
         <v>8</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>5</v>
@@ -5331,13 +5636,13 @@
     </row>
     <row r="49" spans="1:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B49" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="B49" s="10" t="s">
-        <v>168</v>
-      </c>
       <c r="C49" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -5349,7 +5654,7 @@
         <v>2</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>3</v>
@@ -5361,7 +5666,7 @@
         <v>8</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>5</v>
@@ -5369,13 +5674,13 @@
     </row>
     <row r="50" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="C50" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D50" s="4">
         <v>2</v>
@@ -5387,10 +5692,10 @@
         <v>1</v>
       </c>
       <c r="G50" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="H50" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="I50" s="4" t="s">
         <v>3</v>
@@ -5399,7 +5704,7 @@
         <v>8</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>5</v>
@@ -5407,13 +5712,13 @@
     </row>
     <row r="51" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B51" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="B51" s="10" t="s">
-        <v>172</v>
-      </c>
       <c r="C51" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D51" s="4">
         <v>3</v>
@@ -5425,7 +5730,7 @@
         <v>2</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>3</v>
@@ -5437,7 +5742,7 @@
         <v>8</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>5</v>
@@ -5445,13 +5750,13 @@
     </row>
     <row r="52" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>174</v>
-      </c>
       <c r="C52" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D52" s="4">
         <v>3</v>
@@ -5463,7 +5768,7 @@
         <v>2</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>3</v>
@@ -5475,21 +5780,21 @@
         <v>8</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B53" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="B53" s="10" t="s">
-        <v>176</v>
-      </c>
       <c r="C53" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D53" s="4">
         <v>3</v>
@@ -5501,7 +5806,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>3</v>
@@ -5513,21 +5818,21 @@
         <v>8</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="B54" s="10" t="s">
-        <v>178</v>
-      </c>
       <c r="C54" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D54" s="4">
         <v>3</v>
@@ -5539,7 +5844,7 @@
         <v>2</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>3</v>
@@ -5551,7 +5856,7 @@
         <v>8</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>5</v>
@@ -5559,13 +5864,13 @@
     </row>
     <row r="55" spans="1:12" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B55" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="B55" s="10" t="s">
-        <v>180</v>
-      </c>
       <c r="C55" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D55" s="4">
         <v>3</v>
@@ -5577,7 +5882,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>3</v>
@@ -5589,7 +5894,7 @@
         <v>8</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>5</v>
@@ -5597,13 +5902,13 @@
     </row>
     <row r="56" spans="1:12" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="B56" s="10" t="s">
-        <v>182</v>
-      </c>
       <c r="C56" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D56" s="4">
         <v>3</v>
@@ -5615,7 +5920,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>3</v>
@@ -5627,7 +5932,7 @@
         <v>8</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>5</v>
@@ -5635,13 +5940,13 @@
     </row>
     <row r="57" spans="1:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B57" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B57" s="10" t="s">
-        <v>184</v>
-      </c>
       <c r="C57" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D57" s="4">
         <v>3</v>
@@ -5653,7 +5958,7 @@
         <v>2</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>3</v>
@@ -5665,7 +5970,7 @@
         <v>8</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L57" s="4" t="s">
         <v>5</v>
@@ -5673,13 +5978,13 @@
     </row>
     <row r="58" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="B58" s="10" t="s">
-        <v>186</v>
-      </c>
       <c r="C58" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D58" s="4">
         <v>3</v>
@@ -5691,7 +5996,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>3</v>
@@ -5703,7 +6008,7 @@
         <v>8</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L58" s="4" t="s">
         <v>5</v>
@@ -5711,13 +6016,13 @@
     </row>
     <row r="59" spans="1:12" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B59" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B59" s="10" t="s">
-        <v>188</v>
-      </c>
       <c r="C59" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D59" s="4">
         <v>3</v>
@@ -5729,7 +6034,7 @@
         <v>3</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>3</v>
@@ -5741,7 +6046,7 @@
         <v>8</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L59" s="4" t="s">
         <v>5</v>
@@ -5750,17 +6055,17 @@
     <row r="60" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:12" ht="28.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:12" ht="29.4" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="31.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="29.4" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="28.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="28.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" ht="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="71" ht="29.4" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" ht="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="28.8" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="28.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="74" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" ht="28.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="76" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5776,21 +6081,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816D7012-868E-4BBE-987C-E3C87461A1B8}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -5798,15 +6109,110 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="214.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>253</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="1">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1">
+        <v>34</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="161.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="C3" s="1">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <v>35</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="C4" s="1">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1">
+        <v>21</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" s="1">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
+        <v>39</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5815,15 +6221,484 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A96AD38-DAC3-473B-957C-C9158800A56B}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000F74DC-59C5-4021-9C1C-4214790B450D}">
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="B1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.21875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="55" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="41.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" s="18">
+        <v>36</v>
+      </c>
+      <c r="C2" s="18">
+        <v>62</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="B3" s="1">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1">
+        <v>73</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B4" s="1">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1">
+        <v>54</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="D20" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D22" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="85.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="D23" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C30" s="1">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C31" s="1">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A18:C18"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A96AD38-DAC3-473B-957C-C9158800A56B}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" customWidth="1"/>
+    <col min="6" max="6" width="57.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="171.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="1">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
+        <v>16</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" s="1">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>